<commit_message>
Actualizacion Masiva All Ficheros
</commit_message>
<xml_diff>
--- a/admin/JLCPCB/CPL1disenoAnfuso.xlsx
+++ b/admin/JLCPCB/CPL1disenoAnfuso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ELECTRÓNICA GAMBINO\01 CLIENTES\76 EDUARDO ANFUSO\proyectoEduAnfuso\admin\JLCPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1C99F24-E44D-466F-A0B5-672A53AF86BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654CBF4C-F623-411D-8E4E-6EEDE5EFD8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4212" yWindow="1248" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3516" yWindow="3108" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t>Designator</t>
   </si>
@@ -103,142 +103,301 @@
     <t>C12</t>
   </si>
   <si>
+    <t>L01</t>
+  </si>
+  <si>
+    <t>L02</t>
+  </si>
+  <si>
+    <t>L03</t>
+  </si>
+  <si>
+    <t>L04</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R84</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>Q01</t>
+  </si>
+  <si>
+    <t>Q02</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>Q05</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>PRG</t>
+  </si>
+  <si>
+    <t>Q04</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>ULN2803</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R63</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>R56</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>NODEMCU</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>RELAY1</t>
+  </si>
+  <si>
+    <t>RELAY2</t>
+  </si>
+  <si>
+    <t>RELAY3</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>L01</t>
-  </si>
-  <si>
-    <t>L02</t>
-  </si>
-  <si>
-    <t>L03</t>
-  </si>
-  <si>
-    <t>L04</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R84</t>
-  </si>
-  <si>
-    <t>D33</t>
-  </si>
-  <si>
-    <t>Q01</t>
-  </si>
-  <si>
-    <t>Q02</t>
-  </si>
-  <si>
-    <t>Q03</t>
-  </si>
-  <si>
-    <t>Q05</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>PW</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>D29</t>
-  </si>
-  <si>
-    <t>D28</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>C35</t>
-  </si>
-  <si>
-    <t>PRG</t>
-  </si>
-  <si>
-    <t>DEEP SLEEP</t>
-  </si>
-  <si>
-    <t>LED MQTT</t>
-  </si>
-  <si>
-    <t>LED WI-FI</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
+    <t>BAT1</t>
+  </si>
+  <si>
+    <t>FUENTE</t>
+  </si>
+  <si>
+    <t>RST</t>
   </si>
   <si>
     <t>USBTC1</t>
   </si>
   <si>
-    <t>Q04</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>TOP</t>
+    <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>RELAY4</t>
+  </si>
+  <si>
+    <t>MOSFET</t>
+  </si>
+  <si>
+    <t>RELES</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>WI-FI</t>
+  </si>
+  <si>
+    <t>DEEP-SLEEP</t>
+  </si>
+  <si>
+    <t>LED-MQTT</t>
+  </si>
+  <si>
+    <t>LED-WI-FI</t>
+  </si>
+  <si>
+    <t>ESPA</t>
+  </si>
+  <si>
+    <t>ESPB</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>JP4</t>
   </si>
 </sst>
 </file>
@@ -587,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E68"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -621,33 +780,33 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2">
-        <v>82.41</v>
+        <v>59.600099999999998</v>
       </c>
       <c r="C2" s="2">
-        <v>61.4251</v>
+        <v>74.5899</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2">
-        <v>104.66500000000001</v>
+        <v>6.7000099999999998</v>
       </c>
       <c r="C3" s="2">
-        <v>60.296599999999998</v>
+        <v>52.694299999999998</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2">
         <v>90</v>
@@ -655,50 +814,50 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2">
-        <v>29.200099999999999</v>
+        <v>6.7000099999999998</v>
       </c>
       <c r="C4" s="2">
-        <v>58.53</v>
+        <v>63.494399999999999</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2">
-        <v>13.163600000000001</v>
+        <v>6.7000099999999998</v>
       </c>
       <c r="C5" s="2">
-        <v>44.196300000000001</v>
+        <v>74.294200000000004</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2">
-        <v>13.1364</v>
+        <v>90.700100000000006</v>
       </c>
       <c r="C6" s="2">
-        <v>39.196300000000001</v>
+        <v>37.4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -706,16 +865,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2">
-        <v>13.2636</v>
+        <v>70.399900000000002</v>
       </c>
       <c r="C7" s="2">
-        <v>34.196300000000001</v>
+        <v>37.4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -723,16 +882,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2">
-        <v>13.3636</v>
+        <v>70.399900000000002</v>
       </c>
       <c r="C8" s="2">
-        <v>29.196300000000001</v>
+        <v>21.7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -740,50 +899,50 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>13.163600000000001</v>
+        <v>82.41</v>
       </c>
       <c r="C9" s="2">
-        <v>42.896299999999997</v>
+        <v>61.625</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>13.1364</v>
+        <v>104.66500000000001</v>
       </c>
       <c r="C10" s="2">
-        <v>37.796199999999999</v>
+        <v>60.496400000000001</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B11" s="2">
-        <v>13.2364</v>
+        <v>66.580500000000001</v>
       </c>
       <c r="C11" s="2">
-        <v>32.996099999999998</v>
+        <v>71.319900000000004</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E11" s="2">
         <v>180</v>
@@ -791,50 +950,50 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2">
-        <v>13.336399999999999</v>
+        <v>40.865600000000001</v>
       </c>
       <c r="C12" s="2">
-        <v>27.8963</v>
+        <v>22.286000000000001</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2">
-        <v>29.200099999999999</v>
+        <v>42.299900000000001</v>
       </c>
       <c r="C13" s="2">
-        <v>51.1</v>
+        <v>13.83</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2">
-        <v>29.1</v>
+        <v>29.200099999999999</v>
       </c>
       <c r="C14" s="2">
-        <v>44.4</v>
+        <v>58.53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -842,16 +1001,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2">
-        <v>29.1</v>
+        <v>13.163600000000001</v>
       </c>
       <c r="C15" s="2">
-        <v>37.200099999999999</v>
+        <v>44.196300000000001</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -859,101 +1018,101 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2">
-        <v>38.4</v>
+        <v>13.1364</v>
       </c>
       <c r="C16" s="2">
-        <v>44.336500000000001</v>
+        <v>39.196300000000001</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2">
-        <v>38.500100000000003</v>
+        <v>13.2636</v>
       </c>
       <c r="C17" s="2">
-        <v>37.336500000000001</v>
+        <v>34.196300000000001</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2">
-        <v>38.299900000000001</v>
+        <v>13.3636</v>
       </c>
       <c r="C18" s="2">
-        <v>48.5364</v>
+        <v>29.196300000000001</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E18" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2">
-        <v>38.500100000000003</v>
+        <v>13.163600000000001</v>
       </c>
       <c r="C19" s="2">
-        <v>40.736499999999999</v>
+        <v>42.896299999999997</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2">
-        <v>25.38</v>
+        <v>13.1364</v>
       </c>
       <c r="C20" s="2">
-        <v>67.490099999999998</v>
+        <v>37.796199999999999</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
-        <v>19.5</v>
+        <v>13.2364</v>
       </c>
       <c r="C21" s="2">
-        <v>43.200099999999999</v>
+        <v>32.996099999999998</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E21" s="2">
         <v>180</v>
@@ -961,16 +1120,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2">
-        <v>19.5</v>
+        <v>13.336399999999999</v>
       </c>
       <c r="C22" s="2">
-        <v>38.299900000000001</v>
+        <v>27.8963</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E22" s="2">
         <v>180</v>
@@ -978,135 +1137,135 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2">
-        <v>19.5</v>
+        <v>29.200099999999999</v>
       </c>
       <c r="C23" s="2">
-        <v>33.1</v>
+        <v>51.1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E23" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2">
-        <v>19.5</v>
+        <v>29.1</v>
       </c>
       <c r="C24" s="2">
-        <v>27.9999</v>
+        <v>44.4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E24" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2">
-        <v>33.599899999999998</v>
+        <v>29.1</v>
       </c>
       <c r="C25" s="2">
-        <v>74.363600000000005</v>
+        <v>37.200099999999999</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E25" s="2">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2">
-        <v>31.1</v>
+        <v>38.4</v>
       </c>
       <c r="C26" s="2">
-        <v>74.563500000000005</v>
+        <v>44.336500000000001</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E26" s="2">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2">
-        <v>28.1</v>
+        <v>38.500100000000003</v>
       </c>
       <c r="C27" s="2">
-        <v>74.363600000000005</v>
+        <v>37.336500000000001</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2">
-        <v>25.5001</v>
+        <v>38.299900000000001</v>
       </c>
       <c r="C28" s="2">
-        <v>74.563500000000005</v>
+        <v>48.5364</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2">
-        <v>69.363600000000005</v>
+        <v>38.500100000000003</v>
       </c>
       <c r="C29" s="2">
-        <v>54.1</v>
+        <v>40.736499999999999</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E29" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="B30" s="2">
-        <v>69.363600000000005</v>
+        <v>25.38</v>
       </c>
       <c r="C30" s="2">
-        <v>56.6999</v>
+        <v>67.490099999999998</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -1114,152 +1273,152 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B31" s="2">
-        <v>69.363600000000005</v>
+        <v>19.5</v>
       </c>
       <c r="C31" s="2">
-        <v>59.2</v>
+        <v>43.200099999999999</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B32" s="2">
-        <v>69.363600000000005</v>
+        <v>19.5</v>
       </c>
       <c r="C32" s="2">
-        <v>61.8</v>
+        <v>38.299900000000001</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E32" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2">
-        <v>15.7</v>
+        <v>19.5</v>
       </c>
       <c r="C33" s="2">
-        <v>70.536299999999997</v>
+        <v>33.1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E33" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2">
-        <v>26.900099999999998</v>
+        <v>19.5</v>
       </c>
       <c r="C34" s="2">
-        <v>78.063599999999994</v>
+        <v>27.9999</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E34" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B35" s="2">
-        <v>29.5001</v>
+        <v>33.599899999999998</v>
       </c>
       <c r="C35" s="2">
-        <v>78.0364</v>
+        <v>74.363600000000005</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E35" s="2">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2">
-        <v>32.299900000000001</v>
+        <v>31.1</v>
       </c>
       <c r="C36" s="2">
-        <v>78.0364</v>
+        <v>74.563500000000005</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E36" s="2">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B37" s="2">
-        <v>91.636300000000006</v>
+        <v>28.1</v>
       </c>
       <c r="C37" s="2">
-        <v>58.6999</v>
+        <v>74.363600000000005</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E37" s="2">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2">
-        <v>91.636300000000006</v>
+        <v>25.5001</v>
       </c>
       <c r="C38" s="2">
-        <v>61.600099999999998</v>
+        <v>74.563500000000005</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B39" s="2">
-        <v>104.636</v>
+        <v>116.764</v>
       </c>
       <c r="C39" s="2">
-        <v>66.000100000000003</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E39" s="2">
         <v>0</v>
@@ -1267,16 +1426,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B40" s="2">
-        <v>101.464</v>
+        <v>116.764</v>
       </c>
       <c r="C40" s="2">
-        <v>66.000100000000003</v>
+        <v>72.5</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E40" s="2">
         <v>0</v>
@@ -1284,16 +1443,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2">
-        <v>108.06399999999999</v>
+        <v>116.764</v>
       </c>
       <c r="C41" s="2">
-        <v>66.099900000000005</v>
+        <v>75.000100000000003</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E41" s="2">
         <v>0</v>
@@ -1301,101 +1460,101 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2">
-        <v>91.9</v>
+        <v>116.764</v>
       </c>
       <c r="C42" s="2">
-        <v>64.5</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E42" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2">
-        <v>106.7</v>
+        <v>15.7</v>
       </c>
       <c r="C43" s="2">
-        <v>29.9999</v>
+        <v>70.536299999999997</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E43" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B44" s="2">
-        <v>106.7</v>
+        <v>26.900099999999998</v>
       </c>
       <c r="C44" s="2">
-        <v>34.999899999999997</v>
+        <v>78.063599999999994</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E44" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
-        <v>106.7</v>
+        <v>29.5001</v>
       </c>
       <c r="C45" s="2">
-        <v>39.999899999999997</v>
+        <v>78.0364</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E45" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B46" s="2">
-        <v>118.8</v>
+        <v>32.299900000000001</v>
       </c>
       <c r="C46" s="2">
-        <v>5.59999</v>
+        <v>78.0364</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E46" s="2">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B47" s="2">
-        <v>30.1</v>
+        <v>91.636300000000006</v>
       </c>
       <c r="C47" s="2">
-        <v>6.6274899999999999</v>
+        <v>54.5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E47" s="2">
         <v>180</v>
@@ -1403,186 +1562,186 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B48" s="2">
-        <v>14.674799999999999</v>
+        <v>91.636300000000006</v>
       </c>
       <c r="C48" s="2">
-        <v>11.3</v>
+        <v>57.399900000000002</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E48" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2">
-        <v>40.250100000000003</v>
+        <v>104.636</v>
       </c>
       <c r="C49" s="2">
-        <v>22.5</v>
+        <v>66.2</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E49" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B50" s="2">
-        <v>53.999899999999997</v>
+        <v>101.464</v>
       </c>
       <c r="C50" s="2">
-        <v>22.7</v>
+        <v>66.2</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E50" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B51" s="2">
-        <v>19</v>
+        <v>108.06399999999999</v>
       </c>
       <c r="C51" s="2">
-        <v>76.2</v>
+        <v>66.3001</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E51" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B52" s="2">
-        <v>27.569900000000001</v>
+        <v>91.9</v>
       </c>
       <c r="C52" s="2">
-        <v>24.61</v>
+        <v>60.3001</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E52" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B53" s="2">
-        <v>21</v>
+        <v>106.7</v>
       </c>
       <c r="C53" s="2">
-        <v>6.7991000000000001</v>
+        <v>29.9999</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E53" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B54" s="2">
-        <v>12</v>
+        <v>106.7</v>
       </c>
       <c r="C54" s="2">
-        <v>15.1</v>
+        <v>34.999899999999997</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E54" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B55" s="2">
-        <v>49.349899999999998</v>
+        <v>106.7</v>
       </c>
       <c r="C55" s="2">
-        <v>36.850099999999998</v>
+        <v>39.999899999999997</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E55" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B56" s="2">
-        <v>30.5501</v>
+        <v>118.8</v>
       </c>
       <c r="C56" s="2">
-        <v>17.600000000000001</v>
+        <v>5.59999</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E56" s="2">
-        <v>-180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B57" s="2">
-        <v>22.8</v>
+        <v>21.48</v>
       </c>
       <c r="C57" s="2">
-        <v>17.45</v>
+        <v>7.2074999999999996</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E57" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B58" s="2">
-        <v>38.1</v>
+        <v>55.5</v>
       </c>
       <c r="C58" s="2">
-        <v>11.336399999999999</v>
+        <v>22.227900000000002</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E58" s="2">
         <v>90</v>
@@ -1590,33 +1749,33 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B59" s="2">
-        <v>24.2</v>
+        <v>14.674799999999999</v>
       </c>
       <c r="C59" s="2">
-        <v>73.736500000000007</v>
+        <v>11.3</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E59" s="2">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B60" s="2">
-        <v>71.2</v>
+        <v>27.150099999999998</v>
       </c>
       <c r="C60" s="2">
-        <v>5.4999900000000004</v>
+        <v>20.3</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E60" s="2">
         <v>90</v>
@@ -1624,138 +1783,1039 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B61" s="2">
-        <v>80.490099999999998</v>
+        <v>37.4</v>
       </c>
       <c r="C61" s="2">
-        <v>5.4600099999999996</v>
+        <v>30.4</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E61" s="2">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B62" s="2">
-        <v>52.201799999999999</v>
+        <v>19</v>
       </c>
       <c r="C62" s="2">
-        <v>76.000100000000003</v>
+        <v>76.2</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B63" s="2">
-        <v>40.998100000000001</v>
+        <v>26.470099999999999</v>
       </c>
       <c r="C63" s="2">
-        <v>76.000100000000003</v>
+        <v>30.4099</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E63" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="B64" s="2">
-        <v>1.5</v>
+        <v>48.349899999999998</v>
       </c>
       <c r="C64" s="2">
-        <v>3.7999900000000002</v>
+        <v>55.999899999999997</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E64" s="2">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B65" s="2">
-        <v>13.945499999999999</v>
+        <v>29.979900000000001</v>
       </c>
       <c r="C65" s="2">
-        <v>7.8000100000000003</v>
+        <v>7.4099899999999996</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E65" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B66" s="2">
-        <v>8.6000099999999993</v>
+        <v>12</v>
       </c>
       <c r="C66" s="2">
-        <v>3.3500100000000002</v>
+        <v>15.1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E66" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="B67" s="2">
-        <v>106.8</v>
+        <v>49.349899999999998</v>
       </c>
       <c r="C67" s="2">
-        <v>44.999899999999997</v>
+        <v>36.850099999999998</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E67" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="2">
+        <v>39.250100000000003</v>
+      </c>
+      <c r="C68" s="2">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="2">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="2">
+        <v>14.85</v>
+      </c>
+      <c r="C69" s="2">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="2">
+        <v>86.2</v>
+      </c>
+      <c r="C70" s="2">
+        <v>7.1332100000000001</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="2">
+        <v>86.399900000000002</v>
+      </c>
+      <c r="C71" s="2">
+        <v>11.1332</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="2">
+        <v>89.6</v>
+      </c>
+      <c r="C72" s="2">
+        <v>7.1332100000000001</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="2">
+        <v>45.036499999999997</v>
+      </c>
+      <c r="C73" s="2">
+        <v>27.4</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="C74" s="2">
+        <v>73.736500000000007</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="2">
+        <v>77.3001</v>
+      </c>
+      <c r="C75" s="2">
+        <v>11.563599999999999</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="2">
+        <v>80.700100000000006</v>
+      </c>
+      <c r="C76" s="2">
+        <v>11.436400000000001</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="2">
+        <v>74.5</v>
+      </c>
+      <c r="C77" s="2">
+        <v>11.5364</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="2">
+        <v>83.9</v>
+      </c>
+      <c r="C78" s="2">
+        <v>11.436400000000001</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="2">
+        <v>72.000100000000003</v>
+      </c>
+      <c r="C79" s="2">
+        <v>11.436400000000001</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="2">
+        <v>6.7000099999999998</v>
+      </c>
+      <c r="C80" s="2">
+        <v>11.6981</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="2">
+        <v>48.950099999999999</v>
+      </c>
+      <c r="C81" s="2">
+        <v>5.6600099999999998</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" s="2">
+        <v>71.2</v>
+      </c>
+      <c r="C82" s="2">
+        <v>5.4999900000000004</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" s="2">
+        <v>60.710099999999997</v>
+      </c>
+      <c r="C83" s="2">
+        <v>5.6699900000000003</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" s="2">
+        <v>80.490099999999998</v>
+      </c>
+      <c r="C84" s="2">
+        <v>5.4600099999999996</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" s="2">
+        <v>52.201799999999999</v>
+      </c>
+      <c r="C85" s="2">
+        <v>76.000100000000003</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" s="2">
+        <v>40.998100000000001</v>
+      </c>
+      <c r="C86" s="2">
+        <v>76.000100000000003</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C87" s="2">
+        <v>3.7999900000000002</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E87" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="2">
+        <v>13.945499999999999</v>
+      </c>
+      <c r="C88" s="2">
+        <v>7.8000100000000003</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B89" s="2">
+        <v>8.6000099999999993</v>
+      </c>
+      <c r="C89" s="2">
+        <v>3.3500100000000002</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B90" s="2">
+        <v>6.7000099999999998</v>
+      </c>
+      <c r="C90" s="2">
+        <v>40.598100000000002</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E90" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B91" s="2">
+        <v>6.7000099999999998</v>
+      </c>
+      <c r="C91" s="2">
+        <v>27.599900000000002</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E91" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92" s="2">
+        <v>90.700100000000006</v>
+      </c>
+      <c r="C92" s="2">
+        <v>21.7</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="2">
+        <v>110</v>
+      </c>
+      <c r="C93" s="2">
+        <v>4.7999900000000002</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E93" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B94" s="2">
+        <v>106.8</v>
+      </c>
+      <c r="C94" s="2">
+        <v>44.999899999999997</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B95" s="2">
+        <v>106.736</v>
+      </c>
+      <c r="C95" s="2">
+        <v>47.999899999999997</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" s="2">
+        <v>59.69</v>
+      </c>
+      <c r="C96" s="2">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E96" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B97" s="2">
+        <v>59.69</v>
+      </c>
+      <c r="C97" s="2">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E97" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B98" s="2">
+        <v>66.040000000000006</v>
+      </c>
+      <c r="C98" s="2">
+        <v>50.77</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E98" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B99" s="2">
+        <v>67.31</v>
+      </c>
+      <c r="C99" s="2">
+        <v>55.91</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E99" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B100" s="2">
+        <v>91.825299999999999</v>
+      </c>
+      <c r="C100" s="2">
+        <v>63.099899999999998</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" s="2">
+        <v>59.2836</v>
+      </c>
+      <c r="C101" s="2">
+        <v>41.91</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B102" s="2">
+        <v>68.173599999999993</v>
+      </c>
+      <c r="C102" s="2">
+        <v>62.23</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B103" s="2">
+        <v>70.256399999999999</v>
+      </c>
+      <c r="C103" s="2">
+        <v>56.079900000000002</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E103" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B104" s="2">
+        <v>55.473599999999998</v>
+      </c>
+      <c r="C104" s="2">
+        <v>10.16</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E104" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="2">
+        <v>70.256399999999999</v>
+      </c>
+      <c r="C105" s="2">
+        <v>59.889899999999997</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E105" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="2">
+        <v>59.833500000000001</v>
+      </c>
+      <c r="C106" s="2">
+        <v>66.88</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E106" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B107" s="2">
+        <v>56.736499999999999</v>
+      </c>
+      <c r="C107" s="2">
+        <v>67.000100000000003</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="2">
+        <v>115.6</v>
+      </c>
+      <c r="C108" s="2">
+        <v>40.196300000000001</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E108" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" s="2">
+        <v>115.6</v>
+      </c>
+      <c r="C109" s="2">
+        <v>25.296199999999999</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E109" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B110" s="2">
+        <v>93.55</v>
+      </c>
+      <c r="C110" s="2">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E110" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" s="2">
+        <v>93.57</v>
+      </c>
+      <c r="C111" s="2">
+        <v>72.600099999999998</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E111" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B112" s="2">
+        <v>93.749899999999997</v>
+      </c>
+      <c r="C112" s="2">
+        <v>50.299900000000001</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E112" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" s="2">
+        <v>16.8</v>
+      </c>
+      <c r="C113" s="2">
+        <v>57.5</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E113" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B114" s="2">
+        <v>16.8</v>
+      </c>
+      <c r="C114" s="2">
+        <v>54.1</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E114" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B115" s="2">
+        <v>16.8</v>
+      </c>
+      <c r="C115" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E115" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B116" s="2">
+        <v>16.84</v>
+      </c>
+      <c r="C116" s="2">
+        <v>46.900100000000002</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B117" s="2">
+        <v>12.5364</v>
+      </c>
+      <c r="C117" s="2">
+        <v>63.3001</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E117" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B118" s="2">
+        <v>12.5364</v>
+      </c>
+      <c r="C118" s="2">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E118" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B119" s="2">
+        <v>12.5364</v>
+      </c>
+      <c r="C119" s="2">
+        <v>67.3001</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="2">
-        <v>106.736</v>
-      </c>
-      <c r="C68" s="2">
-        <v>47.999899999999997</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E68" s="2">
-        <v>0</v>
+      <c r="B120" s="2">
+        <v>12.5364</v>
+      </c>
+      <c r="C120" s="2">
+        <v>71.3001</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E120" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B121" s="2">
+        <v>64.77</v>
+      </c>
+      <c r="C121" s="2">
+        <v>61.823599999999999</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E121" s="2">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>